<commit_message>
Ajout des liens vers les images de logos
</commit_message>
<xml_diff>
--- a/logo_informations.xlsx
+++ b/logo_informations.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="131">
   <si>
     <t>Nom</t>
   </si>
@@ -23,7 +23,7 @@
     <t>Lien</t>
   </si>
   <si>
-    <t> Couleur Dominante</t>
+    <t>Couleur Dominante</t>
   </si>
   <si>
     <t>Couleur Secondaire</t>
@@ -35,7 +35,7 @@
     <t>La poste</t>
   </si>
   <si>
-    <t>file:///home/isen/Bureau/blind_people/logo/laposte.png</t>
+    <t>/home/isen/Bureau/blind_people/logo/laposte.jpg</t>
   </si>
   <si>
     <t>Bleu</t>
@@ -47,7 +47,7 @@
     <t>Carrefour</t>
   </si>
   <si>
-    <t>file:///home/isen/Bureau/blind_people/logo/carrefour.png</t>
+    <t>/home/isen/Bureau/blind_people/logo/carrefour.jpg</t>
   </si>
   <si>
     <t>Rouge</t>
@@ -56,78 +56,135 @@
     <t>Auchan</t>
   </si>
   <si>
+    <t>/home/isen/Bureau/blind_people/logo/auchan.jpg</t>
+  </si>
+  <si>
     <t>Vert</t>
   </si>
   <si>
     <t>SFR</t>
   </si>
   <si>
+    <t>/home/isen/Bureau/blind_people/logo/sfr.jpg</t>
+  </si>
+  <si>
     <t>Blanc</t>
   </si>
   <si>
     <t>McDonald</t>
   </si>
   <si>
+    <t>/home/isen/Bureau/blind_people/logo/mcdo.jpg</t>
+  </si>
+  <si>
     <t>Casino</t>
   </si>
   <si>
+    <t>/home/isen/Bureau/blind_people/logo/casino.jpg</t>
+  </si>
+  <si>
     <t>Nike</t>
   </si>
   <si>
+    <t>/home/isen/Bureau/blind_people/logo/nike.jpg</t>
+  </si>
+  <si>
     <t>Noir</t>
   </si>
   <si>
     <t>Starbucks</t>
   </si>
   <si>
+    <t>/home/isen/Bureau/blind_people/logo/starbucks.jpg</t>
+  </si>
+  <si>
     <t>Renault</t>
   </si>
   <si>
+    <t>/home/isen/Bureau/blind_people/logo/renault.jpg</t>
+  </si>
+  <si>
     <t>Gris</t>
   </si>
   <si>
     <t>Sport 2000</t>
   </si>
   <si>
+    <t>/home/isen/Bureau/blind_people/logo/sport2000.jpg</t>
+  </si>
+  <si>
     <t>Rouge Noir</t>
   </si>
   <si>
     <t>Decathlon</t>
   </si>
   <si>
+    <t>/home/isen/Bureau/blind_people/logo/decathlon.jpg</t>
+  </si>
+  <si>
     <t>Levis</t>
   </si>
   <si>
+    <t>/home/isen/Bureau/blind_people/logo/levis.jpg</t>
+  </si>
+  <si>
     <t>Adidas</t>
   </si>
   <si>
+    <t>/home/isen/Bureau/blind_people/logo/adidas.jpg</t>
+  </si>
+  <si>
     <t>LCL</t>
   </si>
   <si>
+    <t>/home/isen/Bureau/blind_people/logo/lcl.jpg</t>
+  </si>
+  <si>
     <t>Orange</t>
   </si>
   <si>
+    <t>/home/isen/Bureau/blind_people/logo/orange.jpg</t>
+  </si>
+  <si>
     <t>Bouygues</t>
   </si>
   <si>
+    <t>/home/isen/Bureau/blind_people/logo/bouygues.jpg</t>
+  </si>
+  <si>
     <t>Free</t>
   </si>
   <si>
+    <t>/home/isen/Bureau/blind_people/logo/free.jpg</t>
+  </si>
+  <si>
     <t>Burger King</t>
   </si>
   <si>
+    <t>/home/isen/Bureau/blind_people/logo/burger_king.jpg</t>
+  </si>
+  <si>
     <t>Rouge Jaune</t>
   </si>
   <si>
     <t>KFC</t>
   </si>
   <si>
+    <t>/home/isen/Bureau/blind_people/logo/kfc.jpg</t>
+  </si>
+  <si>
     <t>O'Tacos</t>
   </si>
   <si>
+    <t>/home/isen/Bureau/blind_people/logo/otacos.jpg</t>
+  </si>
+  <si>
     <t>GO Sport</t>
   </si>
   <si>
+    <t>/home/isen/Bureau/blind_people/logo/gosport.jpg</t>
+  </si>
+  <si>
     <t>Gris Blanc</t>
   </si>
   <si>
@@ -137,124 +194,220 @@
     <t>Caisse d'Epargne</t>
   </si>
   <si>
+    <t>/home/isen/Bureau/blind_people/logo/caisseepargne.jpg</t>
+  </si>
+  <si>
     <t>BNP Paribas</t>
   </si>
   <si>
+    <t>/home/isen/Bureau/blind_people/logo/bnpparibas.jpg</t>
+  </si>
+  <si>
     <t>Lacoste</t>
   </si>
   <si>
+    <t>/home/isen/Bureau/blind_people/logo/lacoste.jpg</t>
+  </si>
+  <si>
     <t>Blanc Rouge</t>
   </si>
   <si>
     <t>Maif</t>
   </si>
   <si>
+    <t>/home/isen/Bureau/blind_people/logo/maif.jpg</t>
+  </si>
+  <si>
     <t>Rouge Blanc</t>
   </si>
   <si>
     <t>MMA</t>
   </si>
   <si>
+    <t>/home/isen/Bureau/blind_people/logo/mma.jpg</t>
+  </si>
+  <si>
     <t>Vert Orange</t>
   </si>
   <si>
     <t>Cetelem</t>
   </si>
   <si>
+    <t>/home/isen/Bureau/blind_people/logo/cetelem.jpg</t>
+  </si>
+  <si>
     <t>MAAF</t>
   </si>
   <si>
+    <t>/home/isen/Bureau/blind_people/logo/maaf.jpg</t>
+  </si>
+  <si>
     <t>Axa</t>
   </si>
   <si>
+    <t>/home/isen/Bureau/blind_people/logo/axa.jpg</t>
+  </si>
+  <si>
     <t>Swisslife</t>
   </si>
   <si>
+    <t>/home/isen/Bureau/blind_people/logo/swisslife.jpg</t>
+  </si>
+  <si>
     <t>Noir Blanc</t>
   </si>
   <si>
     <t>Castorama</t>
   </si>
   <si>
+    <t>/home/isen/Bureau/blind_people/logo/castorama.jpg</t>
+  </si>
+  <si>
     <t>Leroy Merlin</t>
   </si>
   <si>
+    <t>/home/isen/Bureau/blind_people/logo/leroymerlin.jpg</t>
+  </si>
+  <si>
     <t>Boulanger</t>
   </si>
   <si>
+    <t>/home/isen/Bureau/blind_people/logo/boulanger.jpg</t>
+  </si>
+  <si>
     <t>Darty</t>
   </si>
   <si>
+    <t>/home/isen/Bureau/blind_people/logo/darty.jpg</t>
+  </si>
+  <si>
     <t>Blanc Noir</t>
   </si>
   <si>
     <t>Fnac</t>
   </si>
   <si>
+    <t>/home/isen/Bureau/blind_people/logo/fnac.jpg</t>
+  </si>
+  <si>
     <t>Charlemagne</t>
   </si>
   <si>
+    <t>/home/isen/Bureau/blind_people/logo/charlemagne.jpg</t>
+  </si>
+  <si>
     <t>Ikea</t>
   </si>
   <si>
+    <t>/home/isen/Bureau/blind_people/logo/ikea.jpg</t>
+  </si>
+  <si>
     <t>Leclerc</t>
   </si>
   <si>
+    <t>/home/isen/Bureau/blind_people/logo/leclerc.jpg</t>
+  </si>
+  <si>
     <t>Orange Blanc</t>
   </si>
   <si>
     <t>Gifi</t>
   </si>
   <si>
+    <t>/home/isen/Bureau/blind_people/logo/gifi.jpg</t>
+  </si>
+  <si>
     <t>Grand Frais</t>
   </si>
   <si>
+    <t>/home/isen/Bureau/blind_people/logo/grandfrais.jpg</t>
+  </si>
+  <si>
     <t>Vert Blanc</t>
   </si>
   <si>
     <t>Jardiland</t>
   </si>
   <si>
+    <t>/home/isen/Bureau/blind_people/logo/jardiland.jpg</t>
+  </si>
+  <si>
     <t>Flunch</t>
   </si>
   <si>
+    <t>/home/isen/Bureau/blind_people/logo/flunch.jpg</t>
+  </si>
+  <si>
     <t>Buffalo Grill</t>
   </si>
   <si>
+    <t>/home/isen/Bureau/blind_people/logo/buffalogrill.jpg</t>
+  </si>
+  <si>
     <t>Courtepaille</t>
   </si>
   <si>
+    <t>/home/isen/Bureau/blind_people/logo/courtepaille.jpg</t>
+  </si>
+  <si>
     <t>Mr.Bricolage</t>
   </si>
   <si>
+    <t>/home/isen/Bureau/blind_people/logo/mrbricolage.jpg</t>
+  </si>
+  <si>
     <t>Animalis</t>
   </si>
   <si>
+    <t>/home/isen/Bureau/blind_people/logo/animalis.jpg</t>
+  </si>
+  <si>
     <t>Intermarché</t>
   </si>
   <si>
+    <t>/home/isen/Bureau/blind_people/logo/intermarche.jpg</t>
+  </si>
+  <si>
     <t>Noir Rouge</t>
   </si>
   <si>
     <t>Optic 2000</t>
   </si>
   <si>
+    <t>/home/isen/Bureau/blind_people/logo/optic2000.jpg</t>
+  </si>
+  <si>
     <t>Violet Jaune</t>
   </si>
   <si>
     <t>Afflelou</t>
   </si>
   <si>
+    <t>/home/isen/Bureau/blind_people/logo/afflelou.jpg</t>
+  </si>
+  <si>
     <t>Optical Center</t>
   </si>
   <si>
+    <t>/home/isen/Bureau/blind_people/logo/opticalcenter.jpg</t>
+  </si>
+  <si>
     <t>Grand Optical</t>
   </si>
   <si>
+    <t>/home/isen/Bureau/blind_people/logo/grandoptical.jpg</t>
+  </si>
+  <si>
     <t>Pharmacie</t>
   </si>
   <si>
+    <t>/home/isen/Bureau/blind_people/logo/pharmcie.jpg</t>
+  </si>
+  <si>
     <t>Peugeot</t>
+  </si>
+  <si>
+    <t>/home/isen/Bureau/blind_people/logo/peugeot.jpg</t>
   </si>
 </sst>
 </file>
@@ -265,7 +418,7 @@
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -286,6 +439,11 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -343,7 +501,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -357,6 +515,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -379,8 +545,8 @@
   </sheetPr>
   <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D50" activeCellId="0" sqref="D50"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A35" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B54" activeCellId="0" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -441,35 +607,41 @@
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="3"/>
+      <c r="B4" s="3" t="s">
+        <v>13</v>
+      </c>
       <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="3"/>
+        <v>15</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="C5" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="3"/>
+        <v>18</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="C6" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>8</v>
@@ -478,113 +650,131 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="3"/>
+        <v>20</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="C7" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="3"/>
+        <v>22</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>23</v>
+      </c>
       <c r="C8" s="2" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="3"/>
+        <v>25</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="C9" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E9" s="3"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="3"/>
+        <v>27</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="C10" s="2" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E10" s="3"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" s="3"/>
+        <v>30</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>31</v>
+      </c>
       <c r="C11" s="2" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="3"/>
+        <v>33</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>34</v>
+      </c>
       <c r="C12" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E12" s="3"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" s="3"/>
+        <v>35</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>36</v>
+      </c>
       <c r="C13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E13" s="3"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" s="3"/>
+        <v>37</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>38</v>
+      </c>
       <c r="C14" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="E14" s="3"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" s="3"/>
+        <v>39</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="C15" s="2" t="s">
         <v>7</v>
       </c>
@@ -595,34 +785,42 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" s="3"/>
+        <v>41</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>42</v>
+      </c>
       <c r="C16" s="1" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E16" s="3"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>30</v>
+        <v>43</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>44</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>31</v>
+        <v>45</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>46</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>11</v>
@@ -630,10 +828,13 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>32</v>
+        <v>47</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>48</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>7</v>
@@ -641,98 +842,125 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>34</v>
+        <v>50</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>51</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>35</v>
+        <v>52</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>53</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>36</v>
+        <v>54</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>55</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>37</v>
+        <v>56</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>39</v>
+        <v>58</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>59</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>40</v>
+        <v>60</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>61</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>41</v>
+        <v>62</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>63</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>43</v>
+        <v>65</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>66</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>44</v>
+        <v>67</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>45</v>
+        <v>68</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>69</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>46</v>
+        <v>70</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>47</v>
+        <v>71</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>72</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>11</v>
@@ -740,40 +968,52 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>48</v>
+        <v>73</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>74</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>49</v>
+        <v>75</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>76</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>50</v>
+        <v>77</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>78</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>51</v>
+        <v>79</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>52</v>
+        <v>80</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>81</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>7</v>
@@ -784,62 +1024,80 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>53</v>
+        <v>82</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>83</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>54</v>
+        <v>84</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>85</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>55</v>
+        <v>86</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>87</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>56</v>
+        <v>88</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>57</v>
+        <v>89</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>90</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>58</v>
+        <v>91</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>92</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>59</v>
+        <v>93</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>94</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>7</v>
@@ -850,18 +1108,24 @@
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>60</v>
+        <v>95</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>96</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>61</v>
+        <v>97</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>62</v>
+        <v>98</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>99</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>8</v>
@@ -872,73 +1136,94 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>63</v>
+        <v>100</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>101</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>64</v>
+        <v>102</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>65</v>
+        <v>103</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>104</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>66</v>
+        <v>105</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>106</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>67</v>
+        <v>107</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>108</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>68</v>
+        <v>109</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>110</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>69</v>
+        <v>111</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>112</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>70</v>
+        <v>113</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>114</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>11</v>
@@ -949,62 +1234,81 @@
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>71</v>
+        <v>115</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>116</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>72</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="D48" s="0"/>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>73</v>
+        <v>118</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>119</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>51</v>
+        <v>79</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>74</v>
+        <v>120</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>75</v>
+        <v>121</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>122</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>37</v>
+        <v>56</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>76</v>
+        <v>123</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>124</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>77</v>
+        <v>125</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>126</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>78</v>
+        <v>127</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>128</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>7</v>
@@ -1012,13 +1316,16 @@
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>79</v>
+        <v>129</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>130</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mise en place de la détection de formes sur les 2 côtés de l'image
</commit_message>
<xml_diff>
--- a/logo_informations.xlsx
+++ b/logo_informations.xlsx
@@ -401,7 +401,7 @@
     <t>Pharmacie</t>
   </si>
   <si>
-    <t>/home/isen/Bureau/blind_people/logo/pharmcie.jpg</t>
+    <t>/home/isen/Bureau/blind_people/logo/pharmacie.jpg</t>
   </si>
   <si>
     <t>Peugeot</t>
@@ -418,7 +418,7 @@
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -439,11 +439,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -501,7 +496,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -515,14 +510,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -546,7 +533,7 @@
   <dimension ref="A1:E54"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A35" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B54" activeCellId="0" sqref="B54"/>
+      <selection pane="topLeft" activeCell="B53" activeCellId="0" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -622,7 +609,7 @@
       <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -637,7 +624,7 @@
       <c r="A6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -652,7 +639,7 @@
       <c r="A7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -667,7 +654,7 @@
       <c r="A8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>23</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -682,7 +669,7 @@
       <c r="A9" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>26</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -697,7 +684,7 @@
       <c r="A10" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>28</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -727,7 +714,7 @@
       <c r="A12" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>34</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -742,7 +729,7 @@
       <c r="A13" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C13" s="2" t="s">
@@ -757,7 +744,7 @@
       <c r="A14" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>38</v>
       </c>
       <c r="C14" s="0" t="s">
@@ -772,7 +759,7 @@
       <c r="A15" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="3" t="s">
         <v>40</v>
       </c>
       <c r="C15" s="2" t="s">
@@ -787,7 +774,7 @@
       <c r="A16" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="3" t="s">
         <v>42</v>
       </c>
       <c r="C16" s="1" t="s">
@@ -802,7 +789,7 @@
       <c r="A17" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="1" t="s">
         <v>44</v>
       </c>
       <c r="C17" s="1" t="s">
@@ -816,7 +803,7 @@
       <c r="A18" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="1" t="s">
         <v>46</v>
       </c>
       <c r="C18" s="1" t="s">
@@ -830,7 +817,7 @@
       <c r="A19" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C19" s="1" t="s">
@@ -844,7 +831,7 @@
       <c r="A20" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="1" t="s">
         <v>51</v>
       </c>
       <c r="C20" s="1" t="s">
@@ -858,7 +845,7 @@
       <c r="A21" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="1" t="s">
         <v>53</v>
       </c>
       <c r="C21" s="1" t="s">
@@ -872,7 +859,7 @@
       <c r="A22" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C22" s="1" t="s">
@@ -886,7 +873,7 @@
       <c r="A23" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="1" t="s">
         <v>59</v>
       </c>
       <c r="C23" s="1" t="s">
@@ -900,7 +887,7 @@
       <c r="A24" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="1" t="s">
         <v>61</v>
       </c>
       <c r="C24" s="1" t="s">
@@ -914,7 +901,7 @@
       <c r="A25" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="1" t="s">
         <v>63</v>
       </c>
       <c r="C25" s="1" t="s">
@@ -928,7 +915,7 @@
       <c r="A26" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="1" t="s">
         <v>66</v>
       </c>
       <c r="C26" s="1" t="s">
@@ -942,7 +929,7 @@
       <c r="A27" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="1" t="s">
         <v>69</v>
       </c>
       <c r="C27" s="1" t="s">
@@ -956,7 +943,7 @@
       <c r="A28" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B28" s="1" t="s">
         <v>72</v>
       </c>
       <c r="C28" s="1" t="s">
@@ -970,7 +957,7 @@
       <c r="A29" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B29" s="1" t="s">
         <v>74</v>
       </c>
       <c r="C29" s="1" t="s">
@@ -984,7 +971,7 @@
       <c r="A30" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="B30" s="1" t="s">
         <v>76</v>
       </c>
       <c r="C30" s="1" t="s">
@@ -998,7 +985,7 @@
       <c r="A31" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B31" s="1" t="s">
         <v>78</v>
       </c>
       <c r="C31" s="1" t="s">
@@ -1012,7 +999,7 @@
       <c r="A32" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B32" s="1" t="s">
         <v>81</v>
       </c>
       <c r="C32" s="1" t="s">
@@ -1026,7 +1013,7 @@
       <c r="A33" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B33" s="1" t="s">
         <v>83</v>
       </c>
       <c r="C33" s="1" t="s">
@@ -1040,7 +1027,7 @@
       <c r="A34" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B34" s="1" t="s">
         <v>85</v>
       </c>
       <c r="C34" s="1" t="s">
@@ -1054,7 +1041,7 @@
       <c r="A35" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B35" s="1" t="s">
         <v>87</v>
       </c>
       <c r="C35" s="1" t="s">
@@ -1068,7 +1055,7 @@
       <c r="A36" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="B36" s="1" t="s">
         <v>90</v>
       </c>
       <c r="C36" s="1" t="s">
@@ -1082,7 +1069,7 @@
       <c r="A37" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="B37" s="1" t="s">
         <v>92</v>
       </c>
       <c r="C37" s="1" t="s">
@@ -1096,7 +1083,7 @@
       <c r="A38" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B38" s="1" t="s">
         <v>94</v>
       </c>
       <c r="C38" s="1" t="s">
@@ -1110,7 +1097,7 @@
       <c r="A39" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="B39" s="1" t="s">
         <v>96</v>
       </c>
       <c r="C39" s="1" t="s">
@@ -1124,7 +1111,7 @@
       <c r="A40" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="B40" s="1" t="s">
         <v>99</v>
       </c>
       <c r="C40" s="1" t="s">
@@ -1138,7 +1125,7 @@
       <c r="A41" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B41" s="5" t="s">
+      <c r="B41" s="1" t="s">
         <v>101</v>
       </c>
       <c r="C41" s="1" t="s">
@@ -1152,7 +1139,7 @@
       <c r="A42" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B42" s="5" t="s">
+      <c r="B42" s="1" t="s">
         <v>104</v>
       </c>
       <c r="C42" s="1" t="s">
@@ -1166,7 +1153,7 @@
       <c r="A43" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B43" s="5" t="s">
+      <c r="B43" s="1" t="s">
         <v>106</v>
       </c>
       <c r="C43" s="1" t="s">
@@ -1180,7 +1167,7 @@
       <c r="A44" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B44" s="5" t="s">
+      <c r="B44" s="1" t="s">
         <v>108</v>
       </c>
       <c r="C44" s="1" t="s">
@@ -1194,7 +1181,7 @@
       <c r="A45" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="B45" s="5" t="s">
+      <c r="B45" s="1" t="s">
         <v>110</v>
       </c>
       <c r="C45" s="1" t="s">
@@ -1208,7 +1195,7 @@
       <c r="A46" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B46" s="5" t="s">
+      <c r="B46" s="1" t="s">
         <v>112</v>
       </c>
       <c r="C46" s="1" t="s">
@@ -1222,7 +1209,7 @@
       <c r="A47" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B47" s="5" t="s">
+      <c r="B47" s="1" t="s">
         <v>114</v>
       </c>
       <c r="C47" s="1" t="s">
@@ -1236,7 +1223,7 @@
       <c r="A48" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B48" s="5" t="s">
+      <c r="B48" s="1" t="s">
         <v>116</v>
       </c>
       <c r="C48" s="1" t="s">
@@ -1262,7 +1249,7 @@
       <c r="A50" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B50" s="5" t="s">
+      <c r="B50" s="1" t="s">
         <v>122</v>
       </c>
       <c r="C50" s="1" t="s">
@@ -1276,7 +1263,7 @@
       <c r="A51" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B51" s="5" t="s">
+      <c r="B51" s="1" t="s">
         <v>124</v>
       </c>
       <c r="C51" s="1" t="s">
@@ -1290,7 +1277,7 @@
       <c r="A52" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="B52" s="5" t="s">
+      <c r="B52" s="1" t="s">
         <v>126</v>
       </c>
       <c r="C52" s="1" t="s">
@@ -1304,21 +1291,21 @@
       <c r="A53" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B53" s="5" t="s">
+      <c r="B53" s="1" t="s">
         <v>128</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B54" s="5" t="s">
+      <c r="B54" s="1" t="s">
         <v>130</v>
       </c>
       <c r="C54" s="1" t="s">

</xml_diff>